<commit_message>
1.表格换行 2.add to experiment table
</commit_message>
<xml_diff>
--- a/resources/experitmet tables.xlsx
+++ b/resources/experitmet tables.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="60">
   <si>
     <t>nDCG@5</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -112,6 +112,126 @@
   <si>
     <t>Before</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Entity1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Entity2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Relation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Score</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sherlock holmes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>united kingdom</t>
+  </si>
+  <si>
+    <t>anthem</t>
+  </si>
+  <si>
+    <t>firstAppearance</t>
+  </si>
+  <si>
+    <t>allegiance</t>
+  </si>
+  <si>
+    <t>apple inc</t>
+  </si>
+  <si>
+    <t>steve jobs</t>
+  </si>
+  <si>
+    <t>foundedBy</t>
+  </si>
+  <si>
+    <t>keyPerson</t>
+  </si>
+  <si>
+    <t>successor</t>
+  </si>
+  <si>
+    <t>adolf hitler</t>
+  </si>
+  <si>
+    <t>world war ii</t>
+  </si>
+  <si>
+    <t>commander</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>battle</t>
+  </si>
+  <si>
+    <t>ceo</t>
+  </si>
+  <si>
+    <t>microsoft</t>
+  </si>
+  <si>
+    <t>redmond</t>
+  </si>
+  <si>
+    <t>locationCity</t>
+  </si>
+  <si>
+    <t>foundationPlace</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>titanic</t>
+  </si>
+  <si>
+    <t>james cameron</t>
+  </si>
+  <si>
+    <t>director</t>
+  </si>
+  <si>
+    <t>cinematography</t>
+  </si>
+  <si>
+    <t>editing</t>
+  </si>
+  <si>
+    <t>leonardo dicaprio</t>
+  </si>
+  <si>
+    <t>starring</t>
+  </si>
+  <si>
+    <t>narrator</t>
+  </si>
+  <si>
+    <t>producer</t>
+  </si>
+  <si>
+    <t>harry potter</t>
+  </si>
+  <si>
+    <t>j k rowling</t>
+  </si>
+  <si>
+    <t>notableWork</t>
+  </si>
+  <si>
+    <t>author</t>
+  </si>
+  <si>
+    <t>coverArtist</t>
   </si>
 </sst>
 </file>
@@ -169,7 +289,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -178,6 +298,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -460,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A19" sqref="A19:D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -660,7 +789,275 @@
         <v>-33.476394849785407</v>
       </c>
     </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="3">
+        <v>7.0793549999999998E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="27" x14ac:dyDescent="0.15">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="3">
+        <v>4.4867869999999999E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="27" x14ac:dyDescent="0.15">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="3">
+        <v>4.3567459999999999E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="27" x14ac:dyDescent="0.15">
+      <c r="A23" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="3">
+        <v>1.5438646E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="27" x14ac:dyDescent="0.15">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" s="3">
+        <v>9.9318410000000003E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="27" x14ac:dyDescent="0.15">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="3">
+        <v>8.0690020000000005E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="27" x14ac:dyDescent="0.15">
+      <c r="A26" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="3">
+        <v>3.7711715999999999E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" s="3">
+        <v>2.2160928999999999E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" s="5">
+        <v>2.44E-5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="27" x14ac:dyDescent="0.15">
+      <c r="A29" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D29" s="3">
+        <v>8.2507291999999996E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="27" x14ac:dyDescent="0.15">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D30" s="3">
+        <v>4.7192255000000002E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D31" s="3">
+        <v>3.6915687000000003E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A32" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D32" s="3">
+        <v>0.12440701799999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="27" x14ac:dyDescent="0.15">
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D33" s="3">
+        <v>9.6447235000000006E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D34" s="3">
+        <v>8.0133909000000003E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A35" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35" s="3">
+        <v>4.9688828999999997E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D36" s="3">
+        <v>3.7266747000000003E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D37" s="3">
+        <v>1.3059708E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="27" x14ac:dyDescent="0.15">
+      <c r="A38" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D38" s="3">
+        <v>1.6964505000000001E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D39" s="3">
+        <v>1.5514061000000001E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="27" x14ac:dyDescent="0.15">
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D40" s="3">
+        <v>1.4906320000000001E-2</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="B26:B28"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1"/>

</xml_diff>

<commit_message>
all revisement after shaw
</commit_message>
<xml_diff>
--- a/resources/experitmet tables.xlsx
+++ b/resources/experitmet tables.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="92">
   <si>
     <t>nDCG@5</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -239,6 +239,101 @@
   </si>
   <si>
     <t>without alpha</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>notation</t>
+  </si>
+  <si>
+    <t>$a$</t>
+  </si>
+  <si>
+    <t>$e_i$</t>
+  </si>
+  <si>
+    <t>$c_i$</t>
+  </si>
+  <si>
+    <t>$n(\cdot)$</t>
+  </si>
+  <si>
+    <t>$h(\cdot)$</t>
+  </si>
+  <si>
+    <t>$c_h$</t>
+  </si>
+  <si>
+    <t>$\bar{C}$</t>
+  </si>
+  <si>
+    <t>$c_l$</t>
+  </si>
+  <si>
+    <t>$\alpha(\cdot,\cdot)$</t>
+  </si>
+  <si>
+    <t>$T_k$</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> meaning </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> attribute </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> entity </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> concept </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CountOf </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> HeadOf </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> head concept </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  head concept set</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> long concept </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> entity pair</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> concept pair</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> joint factor</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> E$A$E tuple with $a_k$ as $A$</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the typicality of the concept pair for an entity pair</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  the typicality of an attribute for a concept pair.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$P(a|\langle c_{1},c_{2}\rangle)$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$\langle c_1,c_2\rangle$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$P(\langle  c_{i},c_{j}\rangle|\langle e_{1},e_{2}\rangle)$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$\langle e_1,e_2\rangle$</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -297,7 +392,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -315,6 +410,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -597,15 +695,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K40"/>
+  <dimension ref="A1:P40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17:P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="13" max="13" width="26.5" customWidth="1"/>
+    <col min="14" max="14" width="15.375" customWidth="1"/>
+    <col min="15" max="15" width="22.125" customWidth="1"/>
+    <col min="16" max="16" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.15">
@@ -788,12 +890,24 @@
         <v>-33.476394849785407</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.15">
       <c r="F17" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="M17" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="N17" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="O17" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="P17" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.15">
       <c r="F18" t="s">
         <v>60</v>
       </c>
@@ -812,8 +926,20 @@
       <c r="K18">
         <v>0.91600000000000004</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="M18" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="N18" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="O18" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="P18" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A19" s="3" t="s">
         <v>22</v>
       </c>
@@ -826,8 +952,20 @@
       <c r="D19" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="M19" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="N19" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="O19" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="P19" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="27" x14ac:dyDescent="0.15">
       <c r="A20" s="5" t="s">
         <v>26</v>
       </c>
@@ -840,8 +978,20 @@
       <c r="D20" s="3">
         <v>7.0793549999999998E-3</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" ht="27" x14ac:dyDescent="0.15">
+      <c r="M20" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="N20" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="O20" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="P20" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="27" x14ac:dyDescent="0.15">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="3" t="s">
@@ -850,8 +1000,20 @@
       <c r="D21" s="3">
         <v>4.4867869999999999E-3</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" ht="27" x14ac:dyDescent="0.15">
+      <c r="M21" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="N21" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="O21" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="P21" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="27" x14ac:dyDescent="0.15">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="3" t="s">
@@ -860,8 +1022,20 @@
       <c r="D22" s="3">
         <v>4.3567459999999999E-3</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" ht="27" x14ac:dyDescent="0.15">
+      <c r="M22" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="N22" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="O22" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="P22" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A23" s="5" t="s">
         <v>31</v>
       </c>
@@ -874,8 +1048,20 @@
       <c r="D23" s="3">
         <v>1.5438646E-2</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" ht="27" x14ac:dyDescent="0.15">
+      <c r="M23" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="N23" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="O23" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="P23" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="3" t="s">
@@ -884,8 +1070,20 @@
       <c r="D24" s="3">
         <v>9.9318410000000003E-3</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" ht="27" x14ac:dyDescent="0.15">
+      <c r="M24" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="N24" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="O24" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="P24" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="27" x14ac:dyDescent="0.15">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="3" t="s">
@@ -895,7 +1093,7 @@
         <v>8.0690020000000005E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="27" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:16" ht="27" x14ac:dyDescent="0.15">
       <c r="A26" s="5" t="s">
         <v>36</v>
       </c>
@@ -909,7 +1107,7 @@
         <v>3.7711715999999999E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="3" t="s">
@@ -919,7 +1117,7 @@
         <v>2.2160928999999999E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="3" t="s">
@@ -929,7 +1127,7 @@
         <v>2.44E-5</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="27" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:16" ht="27" x14ac:dyDescent="0.15">
       <c r="A29" s="5" t="s">
         <v>41</v>
       </c>
@@ -943,7 +1141,7 @@
         <v>8.2507291999999996E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="27" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:16" ht="27" x14ac:dyDescent="0.15">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="3" t="s">
@@ -953,7 +1151,7 @@
         <v>4.7192255000000002E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="3" t="s">
@@ -963,7 +1161,7 @@
         <v>3.6915687000000003E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A32" s="5" t="s">
         <v>46</v>
       </c>
@@ -1067,12 +1265,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="B26:B28"/>
     <mergeCell ref="A38:A40"/>
     <mergeCell ref="B38:B40"/>
     <mergeCell ref="A29:A31"/>
@@ -1081,6 +1273,12 @@
     <mergeCell ref="B32:B34"/>
     <mergeCell ref="A35:A37"/>
     <mergeCell ref="B35:B37"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="B26:B28"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
experiment.tex add: joint conceptualization example
</commit_message>
<xml_diff>
--- a/resources/experitmet tables.xlsx
+++ b/resources/experitmet tables.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="112">
   <si>
     <t>nDCG@5</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -334,6 +334,308 @@
   </si>
   <si>
     <t>$\langle e_1,e_2\rangle$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$e_2$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$e_1$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>barack obama</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>columbia</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>apple</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>steve jobs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ron howard</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Top$\langle c_1,c_2 \rangle$ </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Top $\langle c_1,c_2 \rangle$ with $\alpha$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>film</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,writer&gt;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>book</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,director&gt;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>school</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,politician</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>country</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,leader</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>spa</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>belgium</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>facility</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,country&gt;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>da vinci code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>place</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,country&gt;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>fruit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,entrepreneur&gt;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>company</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,entrepreneur&gt;</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -341,7 +643,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -363,6 +665,23 @@
       <color theme="10"/>
       <name val="宋体"/>
       <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -392,7 +711,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -408,11 +727,14 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -698,12 +1020,15 @@
   <dimension ref="A1:P40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17:P24"/>
+      <selection activeCell="H31" sqref="H31:K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="8" max="8" width="20.875" customWidth="1"/>
+    <col min="9" max="9" width="11.375" customWidth="1"/>
+    <col min="10" max="10" width="17.5" customWidth="1"/>
     <col min="13" max="13" width="26.5" customWidth="1"/>
     <col min="14" max="14" width="15.375" customWidth="1"/>
     <col min="15" max="15" width="22.125" customWidth="1"/>
@@ -894,16 +1219,16 @@
       <c r="F17" t="s">
         <v>61</v>
       </c>
-      <c r="M17" s="6" t="s">
+      <c r="M17" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="N17" s="6" t="s">
+      <c r="N17" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="O17" s="6" t="s">
+      <c r="O17" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="P17" s="6" t="s">
+      <c r="P17" s="5" t="s">
         <v>73</v>
       </c>
     </row>
@@ -926,16 +1251,16 @@
       <c r="K18">
         <v>0.91600000000000004</v>
       </c>
-      <c r="M18" s="6" t="s">
+      <c r="M18" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="N18" s="6" t="s">
+      <c r="N18" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="O18" s="6" t="s">
+      <c r="O18" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="P18" s="6" t="s">
+      <c r="P18" s="5" t="s">
         <v>75</v>
       </c>
     </row>
@@ -952,24 +1277,24 @@
       <c r="D19" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M19" s="6" t="s">
+      <c r="M19" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="N19" s="6" t="s">
+      <c r="N19" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="O19" s="6" t="s">
+      <c r="O19" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="P19" s="6" t="s">
+      <c r="P19" s="5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="27" x14ac:dyDescent="0.15">
-      <c r="A20" s="5" t="s">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A20" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="6" t="s">
         <v>27</v>
       </c>
       <c r="C20" s="3" t="s">
@@ -978,68 +1303,68 @@
       <c r="D20" s="3">
         <v>7.0793549999999998E-3</v>
       </c>
-      <c r="M20" s="6" t="s">
+      <c r="M20" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="N20" s="6" t="s">
+      <c r="N20" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="O20" s="6" t="s">
+      <c r="O20" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="P20" s="6" t="s">
+      <c r="P20" s="5" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="27" x14ac:dyDescent="0.15">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
       <c r="C21" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D21" s="3">
         <v>4.4867869999999999E-3</v>
       </c>
-      <c r="M21" s="6" t="s">
+      <c r="M21" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="N21" s="6" t="s">
+      <c r="N21" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="O21" s="6" t="s">
+      <c r="O21" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="P21" s="6" t="s">
+      <c r="P21" s="5" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="27" x14ac:dyDescent="0.15">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
       <c r="C22" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D22" s="3">
         <v>4.3567459999999999E-3</v>
       </c>
-      <c r="M22" s="6" t="s">
+      <c r="M22" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="N22" s="6" t="s">
+      <c r="N22" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="O22" s="6" t="s">
+      <c r="O22" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="P22" s="6" t="s">
+      <c r="P22" s="5" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="6" t="s">
         <v>32</v>
       </c>
       <c r="C23" s="3" t="s">
@@ -1048,44 +1373,44 @@
       <c r="D23" s="3">
         <v>1.5438646E-2</v>
       </c>
-      <c r="M23" s="6" t="s">
+      <c r="M23" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="N23" s="6" t="s">
+      <c r="N23" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="O23" s="6" t="s">
+      <c r="O23" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="P23" s="6" t="s">
+      <c r="P23" s="5" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="67.5" x14ac:dyDescent="0.15">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
       <c r="C24" s="3" t="s">
         <v>34</v>
       </c>
       <c r="D24" s="3">
         <v>9.9318410000000003E-3</v>
       </c>
-      <c r="M24" s="6" t="s">
+      <c r="M24" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="N24" s="6" t="s">
+      <c r="N24" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="O24" s="6" t="s">
+      <c r="O24" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="P24" s="6" t="s">
+      <c r="P24" s="5" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="27" x14ac:dyDescent="0.15">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
       <c r="C25" s="3" t="s">
         <v>35</v>
       </c>
@@ -1094,10 +1419,10 @@
       </c>
     </row>
     <row r="26" spans="1:16" ht="27" x14ac:dyDescent="0.15">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="6" t="s">
         <v>37</v>
       </c>
       <c r="C26" s="3" t="s">
@@ -1108,8 +1433,8 @@
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
       <c r="C27" s="3" t="s">
         <v>39</v>
       </c>
@@ -1118,8 +1443,8 @@
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
       <c r="C28" s="3" t="s">
         <v>40</v>
       </c>
@@ -1128,10 +1453,10 @@
       </c>
     </row>
     <row r="29" spans="1:16" ht="27" x14ac:dyDescent="0.15">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="6" t="s">
         <v>42</v>
       </c>
       <c r="C29" s="3" t="s">
@@ -1142,8 +1467,8 @@
       </c>
     </row>
     <row r="30" spans="1:16" ht="27" x14ac:dyDescent="0.15">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
       <c r="C30" s="3" t="s">
         <v>44</v>
       </c>
@@ -1152,20 +1477,32 @@
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
       <c r="C31" s="3" t="s">
         <v>45</v>
       </c>
       <c r="D31" s="3">
         <v>3.6915687000000003E-2</v>
       </c>
+      <c r="H31" t="s">
+        <v>93</v>
+      </c>
+      <c r="I31" t="s">
+        <v>92</v>
+      </c>
+      <c r="J31" t="s">
+        <v>99</v>
+      </c>
+      <c r="K31" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="6" t="s">
         <v>47</v>
       </c>
       <c r="C32" s="3" t="s">
@@ -1174,32 +1511,68 @@
       <c r="D32" s="3">
         <v>0.12440701799999999</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="27" x14ac:dyDescent="0.15">
-      <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
+      <c r="H32" t="s">
+        <v>95</v>
+      </c>
+      <c r="I32" t="s">
+        <v>94</v>
+      </c>
+      <c r="J32" t="s">
+        <v>104</v>
+      </c>
+      <c r="K32" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="27" x14ac:dyDescent="0.15">
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
       <c r="C33" s="3" t="s">
         <v>49</v>
       </c>
       <c r="D33" s="3">
         <v>9.6447235000000006E-2</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
+      <c r="H33" t="s">
+        <v>96</v>
+      </c>
+      <c r="I33" t="s">
+        <v>97</v>
+      </c>
+      <c r="J33" t="s">
+        <v>110</v>
+      </c>
+      <c r="K33" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
       <c r="C34" s="3" t="s">
         <v>50</v>
       </c>
       <c r="D34" s="3">
         <v>8.0133909000000003E-2</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A35" s="5" t="s">
+      <c r="H34" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="I34" t="s">
+        <v>98</v>
+      </c>
+      <c r="J34" t="s">
+        <v>102</v>
+      </c>
+      <c r="K34" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A35" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="6" t="s">
         <v>51</v>
       </c>
       <c r="C35" s="3" t="s">
@@ -1208,10 +1581,22 @@
       <c r="D35" s="3">
         <v>4.9688828999999997E-2</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="5"/>
-      <c r="B36" s="5"/>
+      <c r="H35" t="s">
+        <v>105</v>
+      </c>
+      <c r="I35" t="s">
+        <v>106</v>
+      </c>
+      <c r="J35" t="s">
+        <v>107</v>
+      </c>
+      <c r="K35" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
       <c r="C36" s="3" t="s">
         <v>53</v>
       </c>
@@ -1219,9 +1604,9 @@
         <v>3.7266747000000003E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A37" s="6"/>
+      <c r="B37" s="6"/>
       <c r="C37" s="3" t="s">
         <v>54</v>
       </c>
@@ -1229,11 +1614,11 @@
         <v>1.3059708E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="27" x14ac:dyDescent="0.15">
-      <c r="A38" s="5" t="s">
+    <row r="38" spans="1:11" ht="27" x14ac:dyDescent="0.15">
+      <c r="A38" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="6" t="s">
         <v>56</v>
       </c>
       <c r="C38" s="3" t="s">
@@ -1243,9 +1628,9 @@
         <v>1.6964505000000001E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A39" s="5"/>
-      <c r="B39" s="5"/>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
       <c r="C39" s="3" t="s">
         <v>58</v>
       </c>
@@ -1253,9 +1638,9 @@
         <v>1.5514061000000001E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="27" x14ac:dyDescent="0.15">
-      <c r="A40" s="5"/>
-      <c r="B40" s="5"/>
+    <row r="40" spans="1:11" ht="27" x14ac:dyDescent="0.15">
+      <c r="A40" s="6"/>
+      <c r="B40" s="6"/>
       <c r="C40" s="3" t="s">
         <v>59</v>
       </c>
@@ -1265,6 +1650,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="B26:B28"/>
     <mergeCell ref="A38:A40"/>
     <mergeCell ref="B38:B40"/>
     <mergeCell ref="A29:A31"/>
@@ -1273,12 +1664,6 @@
     <mergeCell ref="B32:B34"/>
     <mergeCell ref="A35:A37"/>
     <mergeCell ref="B35:B37"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="B26:B28"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>

</xml_diff>